<commit_message>
Scripting SCD0175 - Penambahan Leads dari Store ke Cart, and Fixing SCD0176 - Validasi BNIMF, SCD0177 - Validasi BNIMF
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0176_Validasi BNIMF.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0176_Validasi BNIMF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840E9DF0-F77E-4F74-835B-73EC22164E22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4902314-B219-4CC1-97D9-DC39FE14548E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="3615" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCD0176" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>SIDEBAR_SUBMENU_SUBMENU</t>
   </si>
@@ -130,10 +130,52 @@
     <t>TEXT8</t>
   </si>
   <si>
-    <t>Ini Alasan</t>
-  </si>
-  <si>
-    <t>UFT Test Add Leads Prospek BNIMF</t>
+    <t>QUERY1</t>
+  </si>
+  <si>
+    <t>EXPL_QUERY1</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT b.Npp, c.KodeOutlet, c.Name, d.KodeOutlet AS KODE_OUTLET_BNI_MULTIFINANCE FROM DigisalesNew..Tbl_Pegawai AS b join DigisalesNew..Tbl_Unit AS c ON b.Unit_Id = c.Id Left Join Digisales_Leads..MappingBniMultifinance as d ON c.KodeOutlet = d.KodeOutlet WHERE Npp = '22914' OR Npp = '49998'</t>
+  </si>
+  <si>
+    <t>Check npp sales memiliki kode outlet untuk bni multifinance</t>
+  </si>
+  <si>
+    <t>Tertarik</t>
+  </si>
+  <si>
+    <t>USER_DB</t>
+  </si>
+  <si>
+    <t>PASSWORD_DB</t>
+  </si>
+  <si>
+    <t>HOSTNAME</t>
+  </si>
+  <si>
+    <t>sa</t>
+  </si>
+  <si>
+    <t>4eFfEJAA!</t>
+  </si>
+  <si>
+    <t>192.168.232.6</t>
+  </si>
+  <si>
+    <t>QUERY2</t>
+  </si>
+  <si>
+    <t>EXPL_QUERY2</t>
+  </si>
+  <si>
+    <t>QUERY3</t>
+  </si>
+  <si>
+    <t>EXPL_QUERY3</t>
+  </si>
+  <si>
+    <t>UFT Test Add Leads Prospek BNIMF 03</t>
   </si>
 </sst>
 </file>
@@ -199,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -236,6 +278,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EAF5E5-8229-45B3-AC11-8AED029F52F4}">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:AB7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,9 +619,16 @@
     <col min="17" max="17" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="90.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.85546875" customWidth="1"/>
+    <col min="23" max="23" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="15.42578125" customWidth="1"/>
+    <col min="27" max="27" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -628,8 +686,35 @@
       <c r="S1" t="s">
         <v>31</v>
       </c>
+      <c r="T1" t="s">
+        <v>32</v>
+      </c>
+      <c r="U1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1" t="s">
+        <v>45</v>
+      </c>
+      <c r="W1" t="s">
+        <v>33</v>
+      </c>
+      <c r="X1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
@@ -662,7 +747,7 @@
       </c>
       <c r="K2" s="7"/>
       <c r="L2" s="12" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="M2" s="14" t="s">
         <v>19</v>
@@ -683,10 +768,29 @@
         <v>26</v>
       </c>
       <c r="S2" s="14" t="s">
-        <v>32</v>
+        <v>36</v>
+      </c>
+      <c r="T2" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="X2" s="17"/>
+      <c r="Y2" s="17"/>
+      <c r="Z2" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB2" s="7" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
       <c r="F3" s="5"/>
       <c r="G3" s="6"/>
@@ -694,7 +798,7 @@
       <c r="O3" s="1"/>
       <c r="P3" s="2"/>
     </row>
-    <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4"/>
       <c r="F4" s="5"/>
       <c r="G4" s="6"/>
@@ -702,12 +806,12 @@
       <c r="P4" s="3"/>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B5" s="4"/>
       <c r="F5" s="5"/>
       <c r="G5" s="6"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="F7" s="5"/>
       <c r="G7" s="6"/>

</xml_diff>